<commit_message>
done floor fly. and some other stuff.
</commit_message>
<xml_diff>
--- a/事件编号.xlsx
+++ b/事件编号.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{22CC6932-7516-4FE7-AEE2-A24EB72B8855}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{0AE871CD-1C88-4D8D-9BF2-B2B4404E6EE6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,13 +20,73 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>黄钥匙</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>空</t>
+    <t>蓝门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蓝钥匙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红钥匙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红血瓶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蓝血瓶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红宝石</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蓝宝石</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>绿史莱姆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红史莱姆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>怪物手册</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑史莱姆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>物品编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>怪物编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>事件编号</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -34,51 +94,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>蓝门</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>蓝钥匙</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>红钥匙</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>红门</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>红血瓶</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>蓝血瓶</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>铁门</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>红宝石</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>蓝宝石</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>绿史莱姆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>红史莱姆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1000+怪物编号</t>
+    <t>楼层传送器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>圣水</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -404,32 +424,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>1001</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -437,90 +451,118 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1002</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>